<commit_message>
Broke AY structure to separate pages for each analysis
</commit_message>
<xml_diff>
--- a/results/palaepaphos/data/pxrf_PP.xlsx
+++ b/results/palaepaphos/data/pxrf_PP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uine\Documents\R\MB\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uine\Documents\R\MB\results\palaepaphos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F1CE9C-F049-4052-8A9F-22A23415B7E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2F7730-ED29-4314-A599-8CBD4F662863}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="0" windowWidth="22455" windowHeight="15495" xr2:uid="{071E5335-377B-4FFD-9872-C5935EC89188}"/>
+    <workbookView xWindow="1560" yWindow="705" windowWidth="20070" windowHeight="15495" xr2:uid="{071E5335-377B-4FFD-9872-C5935EC89188}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5806" uniqueCount="1260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5772" uniqueCount="1226">
   <si>
     <t>soil</t>
   </si>
@@ -3693,108 +3693,6 @@
   </si>
   <si>
     <t>Cal Check</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>P3</t>
-  </si>
-  <si>
-    <t>P4</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>P12</t>
-  </si>
-  <si>
-    <t>P13</t>
-  </si>
-  <si>
-    <t>P14</t>
-  </si>
-  <si>
-    <t>P15</t>
-  </si>
-  <si>
-    <t>P16</t>
-  </si>
-  <si>
-    <t>P17</t>
-  </si>
-  <si>
-    <t>P18</t>
-  </si>
-  <si>
-    <t>P19</t>
-  </si>
-  <si>
-    <t>P20</t>
-  </si>
-  <si>
-    <t>P21</t>
-  </si>
-  <si>
-    <t>P22</t>
-  </si>
-  <si>
-    <t>P23</t>
-  </si>
-  <si>
-    <t>P24</t>
-  </si>
-  <si>
-    <t>P25</t>
-  </si>
-  <si>
-    <t>P26</t>
-  </si>
-  <si>
-    <t>P27</t>
-  </si>
-  <si>
-    <t>P28</t>
-  </si>
-  <si>
-    <t>P29</t>
-  </si>
-  <si>
-    <t>P30</t>
-  </si>
-  <si>
-    <t>P31</t>
-  </si>
-  <si>
-    <t>P32</t>
-  </si>
-  <si>
-    <t>P33</t>
-  </si>
-  <si>
-    <t>P34</t>
   </si>
   <si>
     <t>Type</t>
@@ -4198,8 +4096,8 @@
   <dimension ref="A1:CW92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H84" sqref="H84"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4212,19 +4110,19 @@
   <sheetData>
     <row r="1" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>1254</v>
+        <v>1220</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>1255</v>
+        <v>1221</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>1256</v>
+        <v>1222</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>1123</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>1257</v>
+        <v>1223</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1124</v>
@@ -11741,7 +11639,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>582</v>
@@ -12046,7 +11944,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>582</v>
@@ -12345,7 +12243,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>582</v>
@@ -12644,7 +12542,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>638</v>
@@ -12943,7 +12841,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>638</v>
@@ -13242,7 +13140,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>638</v>
@@ -13541,7 +13439,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>691</v>
@@ -13840,7 +13738,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>691</v>
@@ -14139,7 +14037,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>691</v>
@@ -14438,7 +14336,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>744</v>
@@ -14743,7 +14641,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>744</v>
@@ -15042,7 +14940,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>744</v>
@@ -15341,7 +15239,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>792</v>
@@ -15640,7 +15538,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>792</v>
@@ -15945,7 +15843,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>792</v>
@@ -16244,7 +16142,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>841</v>
@@ -16543,7 +16441,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>841</v>
@@ -16842,7 +16740,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>841</v>
@@ -17141,7 +17039,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>891</v>
@@ -17440,7 +17338,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>891</v>
@@ -17739,7 +17637,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>891</v>
@@ -18044,7 +17942,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>938</v>
@@ -18349,7 +18247,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>938</v>
@@ -18654,7 +18552,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>938</v>
@@ -18953,7 +18851,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>986</v>
@@ -19252,7 +19150,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>986</v>
@@ -19557,7 +19455,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>986</v>
@@ -19856,7 +19754,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>1036</v>
@@ -20161,7 +20059,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>1036</v>
@@ -20466,7 +20364,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>1036</v>
@@ -20771,7 +20669,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>1083</v>
@@ -21076,7 +20974,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>1083</v>
@@ -21381,7 +21279,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1258</v>
+        <v>1224</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>1083</v>
@@ -21686,10 +21584,10 @@
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>1220</v>
+        <v>1225</v>
+      </c>
+      <c r="D59" s="2">
+        <v>1</v>
       </c>
       <c r="AA59">
         <v>0.2107</v>
@@ -21718,10 +21616,10 @@
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>1221</v>
+        <v>1225</v>
+      </c>
+      <c r="D60" s="2">
+        <v>2</v>
       </c>
       <c r="AA60">
         <v>0.21010000000000001</v>
@@ -21750,10 +21648,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>1222</v>
+        <v>1225</v>
+      </c>
+      <c r="D61" s="2">
+        <v>3</v>
       </c>
       <c r="AA61">
         <v>0.20530000000000001</v>
@@ -21782,10 +21680,10 @@
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>1223</v>
+        <v>1225</v>
+      </c>
+      <c r="D62" s="2">
+        <v>4</v>
       </c>
       <c r="AA62">
         <v>0.17319999999999999</v>
@@ -21814,10 +21712,10 @@
         <v>1</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>1224</v>
+        <v>1225</v>
+      </c>
+      <c r="D63" s="2">
+        <v>5</v>
       </c>
       <c r="AA63">
         <v>0.18140000000000001</v>
@@ -21846,10 +21744,10 @@
         <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D64" s="2" t="s">
         <v>1225</v>
+      </c>
+      <c r="D64" s="2">
+        <v>6</v>
       </c>
       <c r="AA64">
         <v>0.18709999999999999</v>
@@ -21878,10 +21776,10 @@
         <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>1226</v>
+        <v>1225</v>
+      </c>
+      <c r="D65" s="2">
+        <v>7</v>
       </c>
       <c r="AA65">
         <v>0.29599999999999999</v>
@@ -21910,10 +21808,10 @@
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>1227</v>
+        <v>1225</v>
+      </c>
+      <c r="D66" s="2">
+        <v>8</v>
       </c>
       <c r="AA66">
         <v>0.1535</v>
@@ -21942,10 +21840,10 @@
         <v>1</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>1228</v>
+        <v>1225</v>
+      </c>
+      <c r="D67" s="2">
+        <v>9</v>
       </c>
       <c r="AA67">
         <v>0.2306</v>
@@ -21974,10 +21872,10 @@
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>1229</v>
+        <v>1225</v>
+      </c>
+      <c r="D68" s="2">
+        <v>10</v>
       </c>
       <c r="AA68">
         <v>0.15440000000000001</v>
@@ -22006,10 +21904,10 @@
         <v>1</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>1230</v>
+        <v>1225</v>
+      </c>
+      <c r="D69" s="2">
+        <v>11</v>
       </c>
       <c r="AA69">
         <v>0.24179999999999999</v>
@@ -22038,10 +21936,10 @@
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>1231</v>
+        <v>1225</v>
+      </c>
+      <c r="D70" s="2">
+        <v>12</v>
       </c>
       <c r="AA70">
         <v>0.2336</v>
@@ -22070,10 +21968,10 @@
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>1232</v>
+        <v>1225</v>
+      </c>
+      <c r="D71" s="2">
+        <v>13</v>
       </c>
       <c r="AA71">
         <v>0.22889999999999999</v>
@@ -22102,10 +22000,10 @@
         <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>1233</v>
+        <v>1225</v>
+      </c>
+      <c r="D72" s="2">
+        <v>14</v>
       </c>
       <c r="AA72">
         <v>0.2283</v>
@@ -22134,10 +22032,10 @@
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>1234</v>
+        <v>1225</v>
+      </c>
+      <c r="D73" s="2">
+        <v>15</v>
       </c>
       <c r="AA73">
         <v>0.29070000000000001</v>
@@ -22166,10 +22064,10 @@
         <v>1</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>1235</v>
+        <v>1225</v>
+      </c>
+      <c r="D74" s="2">
+        <v>16</v>
       </c>
       <c r="AA74">
         <v>0.1895</v>
@@ -22198,10 +22096,10 @@
         <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>1236</v>
+        <v>1225</v>
+      </c>
+      <c r="D75" s="2">
+        <v>17</v>
       </c>
       <c r="AA75">
         <v>0.26779999999999998</v>
@@ -22230,10 +22128,10 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>1237</v>
+        <v>1225</v>
+      </c>
+      <c r="D76" s="2">
+        <v>18</v>
       </c>
       <c r="AA76">
         <v>0.30499999999999999</v>
@@ -22262,10 +22160,10 @@
         <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>1238</v>
+        <v>1225</v>
+      </c>
+      <c r="D77" s="2">
+        <v>19</v>
       </c>
       <c r="AA77">
         <v>0.21179999999999999</v>
@@ -22294,10 +22192,10 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>1239</v>
+        <v>1225</v>
+      </c>
+      <c r="D78" s="2">
+        <v>20</v>
       </c>
       <c r="AA78">
         <v>0.26500000000000001</v>
@@ -22326,10 +22224,10 @@
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>1240</v>
+        <v>1225</v>
+      </c>
+      <c r="D79" s="2">
+        <v>21</v>
       </c>
       <c r="AA79">
         <v>0.25940000000000002</v>
@@ -22358,10 +22256,10 @@
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>1241</v>
+        <v>1225</v>
+      </c>
+      <c r="D80" s="2">
+        <v>22</v>
       </c>
       <c r="AA80">
         <v>0.25490000000000002</v>
@@ -22390,10 +22288,10 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>1242</v>
+        <v>1225</v>
+      </c>
+      <c r="D81" s="2">
+        <v>23</v>
       </c>
       <c r="AA81">
         <v>0.248</v>
@@ -22422,10 +22320,10 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>1243</v>
+        <v>1225</v>
+      </c>
+      <c r="D82" s="2">
+        <v>24</v>
       </c>
       <c r="AA82">
         <v>0.27500000000000002</v>
@@ -22454,10 +22352,10 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>1244</v>
+        <v>1225</v>
+      </c>
+      <c r="D83" s="2">
+        <v>25</v>
       </c>
       <c r="AA83">
         <v>0.2712</v>
@@ -22486,10 +22384,10 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>1245</v>
+        <v>1225</v>
+      </c>
+      <c r="D84" s="2">
+        <v>26</v>
       </c>
       <c r="AA84">
         <v>0.35709999999999997</v>
@@ -22518,10 +22416,10 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>1246</v>
+        <v>1225</v>
+      </c>
+      <c r="D85" s="2">
+        <v>27</v>
       </c>
       <c r="AA85">
         <v>0.29820000000000002</v>
@@ -22550,10 +22448,10 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>1247</v>
+        <v>1225</v>
+      </c>
+      <c r="D86" s="2">
+        <v>28</v>
       </c>
       <c r="AA86">
         <v>0.18729999999999999</v>
@@ -22582,10 +22480,10 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>1248</v>
+        <v>1225</v>
+      </c>
+      <c r="D87" s="2">
+        <v>29</v>
       </c>
       <c r="AA87">
         <v>0.2266</v>
@@ -22614,10 +22512,10 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>1249</v>
+        <v>1225</v>
+      </c>
+      <c r="D88" s="2">
+        <v>30</v>
       </c>
       <c r="AA88">
         <v>0.27450000000000002</v>
@@ -22646,10 +22544,10 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>1250</v>
+        <v>1225</v>
+      </c>
+      <c r="D89" s="2">
+        <v>31</v>
       </c>
       <c r="AA89">
         <v>0.24</v>
@@ -22678,10 +22576,10 @@
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>1251</v>
+        <v>1225</v>
+      </c>
+      <c r="D90" s="2">
+        <v>32</v>
       </c>
       <c r="AA90">
         <v>0.29360000000000003</v>
@@ -22710,10 +22608,10 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>1252</v>
+        <v>1225</v>
+      </c>
+      <c r="D91" s="2">
+        <v>33</v>
       </c>
       <c r="AA91">
         <v>0.27860000000000001</v>
@@ -22742,10 +22640,10 @@
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1259</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>1253</v>
+        <v>1225</v>
+      </c>
+      <c r="D92" s="2">
+        <v>34</v>
       </c>
       <c r="AA92">
         <v>0.2772</v>

</xml_diff>

<commit_message>
Some tweaks to pxrf colors
</commit_message>
<xml_diff>
--- a/results/palaepaphos/data/pxrf_PP.xlsx
+++ b/results/palaepaphos/data/pxrf_PP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uine\Documents\R\MB\results\palaepaphos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2F7730-ED29-4314-A599-8CBD4F662863}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093CC385-1DF4-4C01-80EC-38DA83EB72C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="705" windowWidth="20070" windowHeight="15495" xr2:uid="{071E5335-377B-4FFD-9872-C5935EC89188}"/>
+    <workbookView xWindow="780" yWindow="105" windowWidth="17715" windowHeight="15495" xr2:uid="{071E5335-377B-4FFD-9872-C5935EC89188}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5772" uniqueCount="1226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5772" uniqueCount="1234">
   <si>
     <t>soil</t>
   </si>
@@ -3707,17 +3707,41 @@
     <t>Other name</t>
   </si>
   <si>
-    <t>new</t>
-  </si>
-  <si>
     <t>old</t>
+  </si>
+  <si>
+    <t>mudbrick (old)</t>
+  </si>
+  <si>
+    <t>Hadjuabudllah l1</t>
+  </si>
+  <si>
+    <t>Hadjuabudllah l2</t>
+  </si>
+  <si>
+    <t>Laona soil l1</t>
+  </si>
+  <si>
+    <t>Laona soil l2</t>
+  </si>
+  <si>
+    <t>Laona soil l3</t>
+  </si>
+  <si>
+    <t>LA54:4</t>
+  </si>
+  <si>
+    <t>LA59:2</t>
+  </si>
+  <si>
+    <t>LA54:7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3728,6 +3752,18 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3762,7 +3798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3779,6 +3815,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4096,15 +4133,15 @@
   <dimension ref="A1:CW92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G88" sqref="G88"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -4420,8 +4457,8 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
+      <c r="C2" s="8" t="s">
+        <v>1226</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>2</v>
@@ -4725,8 +4762,8 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>0</v>
+      <c r="C3" s="8" t="s">
+        <v>1226</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>2</v>
@@ -5024,8 +5061,8 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>0</v>
+      <c r="C4" s="8" t="s">
+        <v>1226</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
@@ -5323,8 +5360,8 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>0</v>
+      <c r="C5" s="8" t="s">
+        <v>1227</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>122</v>
@@ -5628,8 +5665,8 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>0</v>
+      <c r="C6" s="8" t="s">
+        <v>1227</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>122</v>
@@ -5927,8 +5964,8 @@
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>0</v>
+      <c r="C7" s="8" t="s">
+        <v>1227</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>122</v>
@@ -6226,8 +6263,8 @@
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>0</v>
+      <c r="C8" s="8" t="s">
+        <v>1228</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>202</v>
@@ -6531,8 +6568,8 @@
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>0</v>
+      <c r="C9" s="8" t="s">
+        <v>1228</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>202</v>
@@ -6830,8 +6867,8 @@
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>0</v>
+      <c r="C10" s="8" t="s">
+        <v>1228</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>202</v>
@@ -7135,8 +7172,8 @@
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>0</v>
+      <c r="C11" s="8" t="s">
+        <v>1229</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>278</v>
@@ -7428,8 +7465,8 @@
       <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>0</v>
+      <c r="C12" s="8" t="s">
+        <v>1229</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>278</v>
@@ -7733,8 +7770,8 @@
       <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>0</v>
+      <c r="C13" s="8" t="s">
+        <v>1229</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>278</v>
@@ -8032,8 +8069,8 @@
       <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>0</v>
+      <c r="C14" s="8" t="s">
+        <v>1230</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>339</v>
@@ -8337,8 +8374,8 @@
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>0</v>
+      <c r="C15" s="8" t="s">
+        <v>1230</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>339</v>
@@ -8636,8 +8673,8 @@
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
+      <c r="C16" s="8" t="s">
+        <v>1230</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>339</v>
@@ -8941,8 +8978,8 @@
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>0</v>
+      <c r="C17" s="8" t="s">
+        <v>1228</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>403</v>
@@ -9234,8 +9271,8 @@
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>0</v>
+      <c r="C18" s="8" t="s">
+        <v>1228</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>403</v>
@@ -9527,8 +9564,8 @@
       <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>0</v>
+      <c r="C19" s="8" t="s">
+        <v>1228</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>403</v>
@@ -9832,8 +9869,8 @@
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>0</v>
+      <c r="C20" s="8" t="s">
+        <v>1229</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>459</v>
@@ -10131,8 +10168,8 @@
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>0</v>
+      <c r="C21" s="8" t="s">
+        <v>1229</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>459</v>
@@ -10430,8 +10467,8 @@
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>0</v>
+      <c r="C22" s="8" t="s">
+        <v>1229</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>459</v>
@@ -10735,8 +10772,8 @@
       <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>0</v>
+      <c r="C23" s="8" t="s">
+        <v>1230</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>517</v>
@@ -11034,8 +11071,8 @@
       <c r="B24" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>0</v>
+      <c r="C24" s="8" t="s">
+        <v>1230</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>517</v>
@@ -11339,8 +11376,8 @@
       <c r="B25" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>0</v>
+      <c r="C25" s="8" t="s">
+        <v>1230</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>517</v>
@@ -11638,8 +11675,8 @@
       <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>1224</v>
+      <c r="C26" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>582</v>
@@ -11943,8 +11980,8 @@
       <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>1224</v>
+      <c r="C27" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>582</v>
@@ -12242,8 +12279,8 @@
       <c r="B28" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>1224</v>
+      <c r="C28" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>582</v>
@@ -12541,8 +12578,8 @@
       <c r="B29" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>1224</v>
+      <c r="C29" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>638</v>
@@ -12840,8 +12877,8 @@
       <c r="B30" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>1224</v>
+      <c r="C30" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>638</v>
@@ -13139,8 +13176,8 @@
       <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>1224</v>
+      <c r="C31" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>638</v>
@@ -13438,8 +13475,8 @@
       <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>1224</v>
+      <c r="C32" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>691</v>
@@ -13737,8 +13774,8 @@
       <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>1224</v>
+      <c r="C33" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>691</v>
@@ -14036,8 +14073,8 @@
       <c r="B34" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>1224</v>
+      <c r="C34" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>691</v>
@@ -14335,8 +14372,8 @@
       <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>1224</v>
+      <c r="C35" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>744</v>
@@ -14640,8 +14677,8 @@
       <c r="B36" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>1224</v>
+      <c r="C36" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>744</v>
@@ -14939,8 +14976,8 @@
       <c r="B37" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>1224</v>
+      <c r="C37" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>744</v>
@@ -15238,8 +15275,8 @@
       <c r="B38" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>1224</v>
+      <c r="C38" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>792</v>
@@ -15537,8 +15574,8 @@
       <c r="B39" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>1224</v>
+      <c r="C39" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>792</v>
@@ -15842,8 +15879,8 @@
       <c r="B40" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>1224</v>
+      <c r="C40" s="8" t="s">
+        <v>1231</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>792</v>
@@ -16141,8 +16178,8 @@
       <c r="B41" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>1224</v>
+      <c r="C41" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>841</v>
@@ -16440,8 +16477,8 @@
       <c r="B42" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>1224</v>
+      <c r="C42" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>841</v>
@@ -16739,8 +16776,8 @@
       <c r="B43" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>1224</v>
+      <c r="C43" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>841</v>
@@ -17038,8 +17075,8 @@
       <c r="B44" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>1224</v>
+      <c r="C44" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>891</v>
@@ -17337,8 +17374,8 @@
       <c r="B45" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>1224</v>
+      <c r="C45" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>891</v>
@@ -17636,8 +17673,8 @@
       <c r="B46" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>1224</v>
+      <c r="C46" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>891</v>
@@ -17941,8 +17978,8 @@
       <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>1224</v>
+      <c r="C47" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>938</v>
@@ -18246,8 +18283,8 @@
       <c r="B48" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>1224</v>
+      <c r="C48" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>938</v>
@@ -18551,8 +18588,8 @@
       <c r="B49" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>1224</v>
+      <c r="C49" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>938</v>
@@ -18850,8 +18887,8 @@
       <c r="B50" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>1224</v>
+      <c r="C50" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>986</v>
@@ -19149,8 +19186,8 @@
       <c r="B51" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>1224</v>
+      <c r="C51" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>986</v>
@@ -19454,8 +19491,8 @@
       <c r="B52" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>1224</v>
+      <c r="C52" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>986</v>
@@ -19753,8 +19790,8 @@
       <c r="B53" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>1224</v>
+      <c r="C53" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>1036</v>
@@ -20058,8 +20095,8 @@
       <c r="B54" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>1224</v>
+      <c r="C54" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>1036</v>
@@ -20363,8 +20400,8 @@
       <c r="B55" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>1224</v>
+      <c r="C55" s="8" t="s">
+        <v>1232</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>1036</v>
@@ -20668,8 +20705,8 @@
       <c r="B56" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>1224</v>
+      <c r="C56" s="8" t="s">
+        <v>1233</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>1083</v>
@@ -20973,8 +21010,8 @@
       <c r="B57" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>1224</v>
+      <c r="C57" s="8" t="s">
+        <v>1233</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>1083</v>
@@ -21278,8 +21315,8 @@
       <c r="B58" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>1224</v>
+      <c r="C58" s="8" t="s">
+        <v>1233</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>1083</v>
@@ -21578,13 +21615,13 @@
     </row>
     <row r="59" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B59" t="s">
         <v>1</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D59" s="2">
         <v>1</v>
@@ -21610,13 +21647,13 @@
     </row>
     <row r="60" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B60" t="s">
         <v>1</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D60" s="2">
         <v>2</v>
@@ -21642,13 +21679,13 @@
     </row>
     <row r="61" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B61" t="s">
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D61" s="2">
         <v>3</v>
@@ -21674,13 +21711,13 @@
     </row>
     <row r="62" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D62" s="2">
         <v>4</v>
@@ -21706,13 +21743,13 @@
     </row>
     <row r="63" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B63" t="s">
         <v>1</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D63" s="2">
         <v>5</v>
@@ -21738,13 +21775,13 @@
     </row>
     <row r="64" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B64" t="s">
         <v>1</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D64" s="2">
         <v>6</v>
@@ -21770,13 +21807,13 @@
     </row>
     <row r="65" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B65" t="s">
         <v>1</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D65" s="2">
         <v>7</v>
@@ -21802,13 +21839,13 @@
     </row>
     <row r="66" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B66" t="s">
         <v>1</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D66" s="2">
         <v>8</v>
@@ -21834,13 +21871,13 @@
     </row>
     <row r="67" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B67" t="s">
         <v>1</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D67" s="2">
         <v>9</v>
@@ -21866,13 +21903,13 @@
     </row>
     <row r="68" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B68" t="s">
         <v>1</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D68" s="2">
         <v>10</v>
@@ -21898,13 +21935,13 @@
     </row>
     <row r="69" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B69" t="s">
         <v>1</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D69" s="2">
         <v>11</v>
@@ -21930,13 +21967,13 @@
     </row>
     <row r="70" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B70" t="s">
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D70" s="2">
         <v>12</v>
@@ -21962,13 +21999,13 @@
     </row>
     <row r="71" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B71" t="s">
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D71" s="2">
         <v>13</v>
@@ -21994,13 +22031,13 @@
     </row>
     <row r="72" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B72" t="s">
         <v>1</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D72" s="2">
         <v>14</v>
@@ -22026,13 +22063,13 @@
     </row>
     <row r="73" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D73" s="2">
         <v>15</v>
@@ -22058,13 +22095,13 @@
     </row>
     <row r="74" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B74" t="s">
         <v>1</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D74" s="2">
         <v>16</v>
@@ -22090,13 +22127,13 @@
     </row>
     <row r="75" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B75" t="s">
         <v>1</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D75" s="2">
         <v>17</v>
@@ -22122,13 +22159,13 @@
     </row>
     <row r="76" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B76" t="s">
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D76" s="2">
         <v>18</v>
@@ -22154,13 +22191,13 @@
     </row>
     <row r="77" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B77" t="s">
         <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D77" s="2">
         <v>19</v>
@@ -22186,13 +22223,13 @@
     </row>
     <row r="78" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B78" t="s">
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D78" s="2">
         <v>20</v>
@@ -22218,13 +22255,13 @@
     </row>
     <row r="79" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B79" t="s">
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D79" s="2">
         <v>21</v>
@@ -22250,13 +22287,13 @@
     </row>
     <row r="80" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B80" t="s">
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D80" s="2">
         <v>22</v>
@@ -22282,13 +22319,13 @@
     </row>
     <row r="81" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B81" t="s">
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D81" s="2">
         <v>23</v>
@@ -22314,13 +22351,13 @@
     </row>
     <row r="82" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D82" s="2">
         <v>24</v>
@@ -22346,13 +22383,13 @@
     </row>
     <row r="83" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B83" t="s">
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D83" s="2">
         <v>25</v>
@@ -22378,13 +22415,13 @@
     </row>
     <row r="84" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B84" t="s">
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D84" s="2">
         <v>26</v>
@@ -22410,13 +22447,13 @@
     </row>
     <row r="85" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B85" t="s">
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D85" s="2">
         <v>27</v>
@@ -22442,13 +22479,13 @@
     </row>
     <row r="86" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B86" t="s">
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D86" s="2">
         <v>28</v>
@@ -22474,13 +22511,13 @@
     </row>
     <row r="87" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B87" t="s">
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D87" s="2">
         <v>29</v>
@@ -22506,13 +22543,13 @@
     </row>
     <row r="88" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D88" s="2">
         <v>30</v>
@@ -22538,13 +22575,13 @@
     </row>
     <row r="89" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B89" t="s">
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D89" s="2">
         <v>31</v>
@@ -22570,13 +22607,13 @@
     </row>
     <row r="90" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B90" t="s">
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D90" s="2">
         <v>32</v>
@@ -22602,13 +22639,13 @@
     </row>
     <row r="91" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B91" t="s">
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D91" s="2">
         <v>33</v>
@@ -22634,13 +22671,13 @@
     </row>
     <row r="92" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>581</v>
+        <v>1225</v>
       </c>
       <c r="B92" t="s">
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="D92" s="2">
         <v>34</v>
@@ -22665,6 +22702,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed old data from PP analysis
</commit_message>
<xml_diff>
--- a/results/palaepaphos/data/pxrf_PP.xlsx
+++ b/results/palaepaphos/data/pxrf_PP.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uine\Documents\R\MB\results\palaepaphos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R\MB\results\palaepaphos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093CC385-1DF4-4C01-80EC-38DA83EB72C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="105" windowWidth="17715" windowHeight="15495" xr2:uid="{071E5335-377B-4FFD-9872-C5935EC89188}"/>
+    <workbookView xWindow="780" yWindow="105" windowWidth="17715" windowHeight="15495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5772" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5670" uniqueCount="1232">
   <si>
     <t>soil</t>
   </si>
@@ -3705,12 +3704,6 @@
   </si>
   <si>
     <t>Other name</t>
-  </si>
-  <si>
-    <t>old</t>
-  </si>
-  <si>
-    <t>mudbrick (old)</t>
   </si>
   <si>
     <t>Hadjuabudllah l1</t>
@@ -3740,18 +3733,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3798,9 +3784,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3815,7 +3800,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4129,12 +4114,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A18BBFC-60BE-4579-9098-33874EBB53A1}">
-  <dimension ref="A1:CW92"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CW58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4142,311 +4127,311 @@
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>1220</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1221</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1222</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>1123</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>1223</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>1124</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>1125</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>1126</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>1127</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>1128</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>1129</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>1130</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>1131</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>1132</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>1133</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>1134</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>1135</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>1136</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>1137</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="4" t="s">
         <v>1138</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="4" t="s">
         <v>1139</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="4" t="s">
         <v>1140</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="4" t="s">
         <v>1141</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="4" t="s">
         <v>1142</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="Y1" s="4" t="s">
         <v>1143</v>
       </c>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="4" t="s">
         <v>1144</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AA1" s="4" t="s">
         <v>1145</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AB1" s="4" t="s">
         <v>1146</v>
       </c>
-      <c r="AC1" s="5" t="s">
+      <c r="AC1" s="4" t="s">
         <v>1147</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AD1" s="4" t="s">
         <v>1148</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AE1" s="4" t="s">
         <v>1149</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AF1" s="4" t="s">
         <v>1150</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" s="4" t="s">
         <v>1151</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AH1" s="4" t="s">
         <v>1152</v>
       </c>
-      <c r="AI1" s="5" t="s">
+      <c r="AI1" s="4" t="s">
         <v>1153</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>1154</v>
       </c>
-      <c r="AK1" s="5" t="s">
+      <c r="AK1" s="4" t="s">
         <v>1155</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AL1" s="4" t="s">
         <v>1156</v>
       </c>
-      <c r="AM1" s="5" t="s">
+      <c r="AM1" s="4" t="s">
         <v>1157</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="AN1" s="4" t="s">
         <v>1158</v>
       </c>
-      <c r="AO1" s="5" t="s">
+      <c r="AO1" s="4" t="s">
         <v>1159</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AP1" s="4" t="s">
         <v>1160</v>
       </c>
-      <c r="AQ1" s="5" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>1161</v>
       </c>
-      <c r="AR1" s="5" t="s">
+      <c r="AR1" s="4" t="s">
         <v>1162</v>
       </c>
-      <c r="AS1" s="5" t="s">
+      <c r="AS1" s="4" t="s">
         <v>1163</v>
       </c>
-      <c r="AT1" s="5" t="s">
+      <c r="AT1" s="4" t="s">
         <v>1164</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AU1" s="4" t="s">
         <v>1165</v>
       </c>
-      <c r="AV1" s="5" t="s">
+      <c r="AV1" s="4" t="s">
         <v>1166</v>
       </c>
-      <c r="AW1" s="5" t="s">
+      <c r="AW1" s="4" t="s">
         <v>1167</v>
       </c>
-      <c r="AX1" s="5" t="s">
+      <c r="AX1" s="4" t="s">
         <v>1168</v>
       </c>
-      <c r="AY1" s="5" t="s">
+      <c r="AY1" s="4" t="s">
         <v>1169</v>
       </c>
-      <c r="AZ1" s="5" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>1170</v>
       </c>
-      <c r="BA1" s="5" t="s">
+      <c r="BA1" s="4" t="s">
         <v>1171</v>
       </c>
-      <c r="BB1" s="5" t="s">
+      <c r="BB1" s="4" t="s">
         <v>1172</v>
       </c>
-      <c r="BC1" s="5" t="s">
+      <c r="BC1" s="4" t="s">
         <v>1173</v>
       </c>
-      <c r="BD1" s="5" t="s">
+      <c r="BD1" s="4" t="s">
         <v>1174</v>
       </c>
-      <c r="BE1" s="5" t="s">
+      <c r="BE1" s="4" t="s">
         <v>1175</v>
       </c>
-      <c r="BF1" s="5" t="s">
+      <c r="BF1" s="4" t="s">
         <v>1176</v>
       </c>
-      <c r="BG1" s="5" t="s">
+      <c r="BG1" s="4" t="s">
         <v>1177</v>
       </c>
-      <c r="BH1" s="5" t="s">
+      <c r="BH1" s="4" t="s">
         <v>1178</v>
       </c>
-      <c r="BI1" s="5" t="s">
+      <c r="BI1" s="4" t="s">
         <v>1179</v>
       </c>
-      <c r="BJ1" s="5" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>1180</v>
       </c>
-      <c r="BK1" s="5" t="s">
+      <c r="BK1" s="4" t="s">
         <v>1181</v>
       </c>
-      <c r="BL1" s="5" t="s">
+      <c r="BL1" s="4" t="s">
         <v>1182</v>
       </c>
-      <c r="BM1" s="5" t="s">
+      <c r="BM1" s="4" t="s">
         <v>1183</v>
       </c>
-      <c r="BN1" s="5" t="s">
+      <c r="BN1" s="4" t="s">
         <v>1184</v>
       </c>
-      <c r="BO1" s="5" t="s">
+      <c r="BO1" s="4" t="s">
         <v>1185</v>
       </c>
-      <c r="BP1" s="5" t="s">
+      <c r="BP1" s="4" t="s">
         <v>1186</v>
       </c>
-      <c r="BQ1" s="5" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>1187</v>
       </c>
-      <c r="BR1" s="5" t="s">
+      <c r="BR1" s="4" t="s">
         <v>1188</v>
       </c>
-      <c r="BS1" s="5" t="s">
+      <c r="BS1" s="4" t="s">
         <v>1189</v>
       </c>
-      <c r="BT1" s="5" t="s">
+      <c r="BT1" s="4" t="s">
         <v>1190</v>
       </c>
-      <c r="BU1" s="5" t="s">
+      <c r="BU1" s="4" t="s">
         <v>1191</v>
       </c>
-      <c r="BV1" s="5" t="s">
+      <c r="BV1" s="4" t="s">
         <v>1192</v>
       </c>
-      <c r="BW1" s="5" t="s">
+      <c r="BW1" s="4" t="s">
         <v>1193</v>
       </c>
-      <c r="BX1" s="5" t="s">
+      <c r="BX1" s="4" t="s">
         <v>1194</v>
       </c>
-      <c r="BY1" s="5" t="s">
+      <c r="BY1" s="4" t="s">
         <v>1195</v>
       </c>
-      <c r="BZ1" s="5" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>1196</v>
       </c>
-      <c r="CA1" s="5" t="s">
+      <c r="CA1" s="4" t="s">
         <v>1197</v>
       </c>
-      <c r="CB1" s="5" t="s">
+      <c r="CB1" s="4" t="s">
         <v>1198</v>
       </c>
-      <c r="CC1" s="5" t="s">
+      <c r="CC1" s="4" t="s">
         <v>1199</v>
       </c>
-      <c r="CD1" s="5" t="s">
+      <c r="CD1" s="4" t="s">
         <v>1200</v>
       </c>
-      <c r="CE1" s="5" t="s">
+      <c r="CE1" s="4" t="s">
         <v>1201</v>
       </c>
-      <c r="CF1" s="5" t="s">
+      <c r="CF1" s="4" t="s">
         <v>1202</v>
       </c>
-      <c r="CG1" s="5" t="s">
+      <c r="CG1" s="4" t="s">
         <v>1203</v>
       </c>
-      <c r="CH1" s="5" t="s">
+      <c r="CH1" s="4" t="s">
         <v>1204</v>
       </c>
-      <c r="CI1" s="5" t="s">
+      <c r="CI1" s="4" t="s">
         <v>1205</v>
       </c>
-      <c r="CJ1" s="5" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>1206</v>
       </c>
-      <c r="CK1" s="5" t="s">
+      <c r="CK1" s="4" t="s">
         <v>1207</v>
       </c>
-      <c r="CL1" s="5" t="s">
+      <c r="CL1" s="4" t="s">
         <v>1208</v>
       </c>
-      <c r="CM1" s="5" t="s">
+      <c r="CM1" s="4" t="s">
         <v>1209</v>
       </c>
-      <c r="CN1" s="5" t="s">
+      <c r="CN1" s="4" t="s">
         <v>1210</v>
       </c>
-      <c r="CO1" s="5" t="s">
+      <c r="CO1" s="4" t="s">
         <v>1211</v>
       </c>
-      <c r="CP1" s="5" t="s">
+      <c r="CP1" s="4" t="s">
         <v>1212</v>
       </c>
-      <c r="CQ1" s="5" t="s">
+      <c r="CQ1" s="4" t="s">
         <v>1213</v>
       </c>
-      <c r="CR1" s="5" t="s">
+      <c r="CR1" s="4" t="s">
         <v>1214</v>
       </c>
-      <c r="CS1" s="5" t="s">
+      <c r="CS1" s="4" t="s">
         <v>1215</v>
       </c>
-      <c r="CT1" s="5" t="s">
+      <c r="CT1" s="4" t="s">
         <v>1216</v>
       </c>
-      <c r="CU1" s="5" t="s">
+      <c r="CU1" s="4" t="s">
         <v>1217</v>
       </c>
-      <c r="CV1" s="5" t="s">
+      <c r="CV1" s="4" t="s">
         <v>1218</v>
       </c>
-      <c r="CW1" s="5" t="s">
+      <c r="CW1" s="4" t="s">
         <v>1219</v>
       </c>
     </row>
@@ -4457,13 +4442,13 @@
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="7" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F2">
@@ -4478,7 +4463,7 @@
       <c r="I2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>7.5</v>
       </c>
       <c r="K2" t="s">
@@ -4762,13 +4747,13 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="7" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F3">
@@ -4783,7 +4768,7 @@
       <c r="I3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>7.5</v>
       </c>
       <c r="K3" t="s">
@@ -5061,13 +5046,13 @@
       <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>1226</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="7" t="s">
+        <v>1224</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F4">
@@ -5082,7 +5067,7 @@
       <c r="I4" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>7.5</v>
       </c>
       <c r="K4" t="s">
@@ -5360,13 +5345,13 @@
       <c r="B5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>1227</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="7" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F5">
@@ -5381,7 +5366,7 @@
       <c r="I5" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>7.541666666666667</v>
       </c>
       <c r="K5" t="s">
@@ -5665,13 +5650,13 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>1227</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="7" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F6">
@@ -5686,7 +5671,7 @@
       <c r="I6" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>7.5</v>
       </c>
       <c r="K6" t="s">
@@ -5964,13 +5949,13 @@
       <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>1227</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="7" t="s">
+        <v>1225</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>122</v>
       </c>
       <c r="F7">
@@ -5985,7 +5970,7 @@
       <c r="I7" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>7.5</v>
       </c>
       <c r="K7" t="s">
@@ -6263,13 +6248,13 @@
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>1228</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>202</v>
       </c>
       <c r="F8">
@@ -6284,7 +6269,7 @@
       <c r="I8" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>7.5</v>
       </c>
       <c r="K8" t="s">
@@ -6568,13 +6553,13 @@
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>1228</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>202</v>
       </c>
       <c r="F9">
@@ -6589,7 +6574,7 @@
       <c r="I9" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>7.5</v>
       </c>
       <c r="K9" t="s">
@@ -6867,13 +6852,13 @@
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>1228</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>202</v>
       </c>
       <c r="F10">
@@ -6888,7 +6873,7 @@
       <c r="I10" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>7.5</v>
       </c>
       <c r="K10" t="s">
@@ -7172,13 +7157,13 @@
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>278</v>
       </c>
       <c r="F11">
@@ -7193,7 +7178,7 @@
       <c r="I11" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>7.5</v>
       </c>
       <c r="K11" t="s">
@@ -7465,13 +7450,13 @@
       <c r="B12" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>278</v>
       </c>
       <c r="F12">
@@ -7486,7 +7471,7 @@
       <c r="I12" t="s">
         <v>5</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>7.5</v>
       </c>
       <c r="K12" t="s">
@@ -7770,13 +7755,13 @@
       <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>278</v>
       </c>
       <c r="F13">
@@ -7791,7 +7776,7 @@
       <c r="I13" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <v>7.5</v>
       </c>
       <c r="K13" t="s">
@@ -8069,13 +8054,13 @@
       <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>1230</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>339</v>
       </c>
       <c r="F14">
@@ -8090,7 +8075,7 @@
       <c r="I14" t="s">
         <v>5</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="3">
         <v>7.5</v>
       </c>
       <c r="K14" t="s">
@@ -8374,13 +8359,13 @@
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>1230</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>339</v>
       </c>
       <c r="F15">
@@ -8395,7 +8380,7 @@
       <c r="I15" t="s">
         <v>5</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <v>7.5</v>
       </c>
       <c r="K15" t="s">
@@ -8673,13 +8658,13 @@
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>1230</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>339</v>
       </c>
       <c r="F16">
@@ -8694,7 +8679,7 @@
       <c r="I16" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="3">
         <v>7.5</v>
       </c>
       <c r="K16" t="s">
@@ -8978,13 +8963,13 @@
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>1228</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>403</v>
       </c>
       <c r="F17">
@@ -8999,7 +8984,7 @@
       <c r="I17" t="s">
         <v>5</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="3">
         <v>7.5</v>
       </c>
       <c r="K17" t="s">
@@ -9271,13 +9256,13 @@
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>1228</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>403</v>
       </c>
       <c r="F18">
@@ -9292,7 +9277,7 @@
       <c r="I18" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="3">
         <v>7.5</v>
       </c>
       <c r="K18" t="s">
@@ -9564,13 +9549,13 @@
       <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>1228</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="C19" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>403</v>
       </c>
       <c r="F19">
@@ -9585,7 +9570,7 @@
       <c r="I19" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="3">
         <v>7.5</v>
       </c>
       <c r="K19" t="s">
@@ -9869,13 +9854,13 @@
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="C20" s="7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>459</v>
       </c>
       <c r="F20">
@@ -9890,7 +9875,7 @@
       <c r="I20" t="s">
         <v>5</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="3">
         <v>7.5</v>
       </c>
       <c r="K20" t="s">
@@ -10168,13 +10153,13 @@
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C21" s="7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>459</v>
       </c>
       <c r="F21">
@@ -10189,7 +10174,7 @@
       <c r="I21" t="s">
         <v>5</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="3">
         <v>7.5</v>
       </c>
       <c r="K21" t="s">
@@ -10467,13 +10452,13 @@
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>1229</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="C22" s="7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>459</v>
       </c>
       <c r="F22">
@@ -10488,7 +10473,7 @@
       <c r="I22" t="s">
         <v>5</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="3">
         <v>7.5</v>
       </c>
       <c r="K22" t="s">
@@ -10772,13 +10757,13 @@
       <c r="B23" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>1230</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="C23" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>517</v>
       </c>
       <c r="F23">
@@ -10793,7 +10778,7 @@
       <c r="I23" t="s">
         <v>5</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="3">
         <v>7.5</v>
       </c>
       <c r="K23" t="s">
@@ -11071,13 +11056,13 @@
       <c r="B24" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>1230</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="C24" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>517</v>
       </c>
       <c r="F24">
@@ -11092,7 +11077,7 @@
       <c r="I24" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="3">
         <v>7.5</v>
       </c>
       <c r="K24" t="s">
@@ -11376,13 +11361,13 @@
       <c r="B25" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>1230</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="C25" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>517</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>517</v>
       </c>
       <c r="F25">
@@ -11397,7 +11382,7 @@
       <c r="I25" t="s">
         <v>5</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="3">
         <v>7.5</v>
       </c>
       <c r="K25" t="s">
@@ -11675,13 +11660,13 @@
       <c r="B26" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="C26" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="E26" s="2" t="s">
         <v>582</v>
       </c>
       <c r="F26">
@@ -11696,7 +11681,7 @@
       <c r="I26" t="s">
         <v>5</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="3">
         <v>7.5</v>
       </c>
       <c r="K26" t="s">
@@ -11980,13 +11965,13 @@
       <c r="B27" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="C27" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>582</v>
       </c>
       <c r="F27">
@@ -12001,7 +11986,7 @@
       <c r="I27" t="s">
         <v>5</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="3">
         <v>7.5</v>
       </c>
       <c r="K27" t="s">
@@ -12279,13 +12264,13 @@
       <c r="B28" t="s">
         <v>1</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="C28" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>582</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E28" s="2" t="s">
         <v>582</v>
       </c>
       <c r="F28">
@@ -12300,7 +12285,7 @@
       <c r="I28" t="s">
         <v>5</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="3">
         <v>7.5</v>
       </c>
       <c r="K28" t="s">
@@ -12578,13 +12563,13 @@
       <c r="B29" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D29" s="2" t="s">
+      <c r="C29" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="2" t="s">
         <v>638</v>
       </c>
       <c r="F29">
@@ -12599,7 +12584,7 @@
       <c r="I29" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="3">
         <v>7.5</v>
       </c>
       <c r="K29" t="s">
@@ -12877,13 +12862,13 @@
       <c r="B30" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D30" s="2" t="s">
+      <c r="C30" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E30" s="2" t="s">
         <v>638</v>
       </c>
       <c r="F30">
@@ -12898,7 +12883,7 @@
       <c r="I30" t="s">
         <v>5</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30" s="3">
         <v>7.5</v>
       </c>
       <c r="K30" t="s">
@@ -13176,13 +13161,13 @@
       <c r="B31" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D31" s="2" t="s">
+      <c r="C31" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>638</v>
       </c>
       <c r="F31">
@@ -13197,7 +13182,7 @@
       <c r="I31" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31" s="3">
         <v>7.5</v>
       </c>
       <c r="K31" t="s">
@@ -13475,13 +13460,13 @@
       <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="C32" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="E32" s="2" t="s">
         <v>691</v>
       </c>
       <c r="F32">
@@ -13496,7 +13481,7 @@
       <c r="I32" t="s">
         <v>5</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="3">
         <v>7.5</v>
       </c>
       <c r="K32" t="s">
@@ -13774,13 +13759,13 @@
       <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D33" s="2" t="s">
+      <c r="C33" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>691</v>
       </c>
       <c r="F33">
@@ -13795,7 +13780,7 @@
       <c r="I33" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33" s="3">
         <v>7.5</v>
       </c>
       <c r="K33" t="s">
@@ -14073,13 +14058,13 @@
       <c r="B34" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D34" s="2" t="s">
+      <c r="C34" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>691</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>691</v>
       </c>
       <c r="F34">
@@ -14094,7 +14079,7 @@
       <c r="I34" t="s">
         <v>5</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="3">
         <v>7.5</v>
       </c>
       <c r="K34" t="s">
@@ -14372,13 +14357,13 @@
       <c r="B35" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="C35" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>744</v>
       </c>
       <c r="F35">
@@ -14393,7 +14378,7 @@
       <c r="I35" t="s">
         <v>5</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="3">
         <v>7.5</v>
       </c>
       <c r="K35" t="s">
@@ -14677,13 +14662,13 @@
       <c r="B36" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="C36" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>744</v>
       </c>
       <c r="F36">
@@ -14698,7 +14683,7 @@
       <c r="I36" t="s">
         <v>5</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="3">
         <v>7.5</v>
       </c>
       <c r="K36" t="s">
@@ -14976,13 +14961,13 @@
       <c r="B37" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="C37" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>744</v>
       </c>
       <c r="F37">
@@ -14997,7 +14982,7 @@
       <c r="I37" t="s">
         <v>5</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="3">
         <v>7.5</v>
       </c>
       <c r="K37" t="s">
@@ -15275,13 +15260,13 @@
       <c r="B38" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="C38" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>792</v>
       </c>
       <c r="F38">
@@ -15296,7 +15281,7 @@
       <c r="I38" t="s">
         <v>5</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="3">
         <v>7.5</v>
       </c>
       <c r="K38" t="s">
@@ -15574,13 +15559,13 @@
       <c r="B39" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="C39" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>792</v>
       </c>
       <c r="F39">
@@ -15595,7 +15580,7 @@
       <c r="I39" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="3">
         <v>7.5</v>
       </c>
       <c r="K39" t="s">
@@ -15879,13 +15864,13 @@
       <c r="B40" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>1231</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C40" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="2" t="s">
         <v>792</v>
       </c>
       <c r="F40">
@@ -15900,7 +15885,7 @@
       <c r="I40" t="s">
         <v>5</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40" s="3">
         <v>7.5</v>
       </c>
       <c r="K40" t="s">
@@ -16178,13 +16163,13 @@
       <c r="B41" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="C41" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>841</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>841</v>
       </c>
       <c r="F41">
@@ -16199,7 +16184,7 @@
       <c r="I41" t="s">
         <v>5</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41" s="3">
         <v>7.5</v>
       </c>
       <c r="K41" t="s">
@@ -16477,13 +16462,13 @@
       <c r="B42" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="C42" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>841</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="2" t="s">
         <v>841</v>
       </c>
       <c r="F42">
@@ -16498,7 +16483,7 @@
       <c r="I42" t="s">
         <v>5</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="3">
         <v>7.5</v>
       </c>
       <c r="K42" t="s">
@@ -16776,13 +16761,13 @@
       <c r="B43" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="C43" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>841</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>841</v>
       </c>
       <c r="F43">
@@ -16797,7 +16782,7 @@
       <c r="I43" t="s">
         <v>5</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="3">
         <v>7.5</v>
       </c>
       <c r="K43" t="s">
@@ -17075,13 +17060,13 @@
       <c r="B44" t="s">
         <v>1</v>
       </c>
-      <c r="C44" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="C44" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>891</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="2" t="s">
         <v>891</v>
       </c>
       <c r="F44">
@@ -17096,7 +17081,7 @@
       <c r="I44" t="s">
         <v>5</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44" s="3">
         <v>7.5</v>
       </c>
       <c r="K44" t="s">
@@ -17374,13 +17359,13 @@
       <c r="B45" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D45" s="2" t="s">
+      <c r="C45" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>891</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>891</v>
       </c>
       <c r="F45">
@@ -17395,7 +17380,7 @@
       <c r="I45" t="s">
         <v>5</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45" s="3">
         <v>7.5</v>
       </c>
       <c r="K45" t="s">
@@ -17673,13 +17658,13 @@
       <c r="B46" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="C46" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>891</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="2" t="s">
         <v>891</v>
       </c>
       <c r="F46">
@@ -17694,7 +17679,7 @@
       <c r="I46" t="s">
         <v>5</v>
       </c>
-      <c r="J46" s="4">
+      <c r="J46" s="3">
         <v>7.5</v>
       </c>
       <c r="K46" t="s">
@@ -17978,13 +17963,13 @@
       <c r="B47" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="C47" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>938</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="2" t="s">
         <v>938</v>
       </c>
       <c r="F47">
@@ -17999,7 +17984,7 @@
       <c r="I47" t="s">
         <v>5</v>
       </c>
-      <c r="J47" s="4">
+      <c r="J47" s="3">
         <v>7.5</v>
       </c>
       <c r="K47" t="s">
@@ -18283,13 +18268,13 @@
       <c r="B48" t="s">
         <v>1</v>
       </c>
-      <c r="C48" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C48" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>938</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="2" t="s">
         <v>938</v>
       </c>
       <c r="F48">
@@ -18304,7 +18289,7 @@
       <c r="I48" t="s">
         <v>5</v>
       </c>
-      <c r="J48" s="4">
+      <c r="J48" s="3">
         <v>7.5</v>
       </c>
       <c r="K48" t="s">
@@ -18588,13 +18573,13 @@
       <c r="B49" t="s">
         <v>1</v>
       </c>
-      <c r="C49" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="C49" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>938</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="E49" s="2" t="s">
         <v>938</v>
       </c>
       <c r="F49">
@@ -18609,7 +18594,7 @@
       <c r="I49" t="s">
         <v>5</v>
       </c>
-      <c r="J49" s="4">
+      <c r="J49" s="3">
         <v>7.5</v>
       </c>
       <c r="K49" t="s">
@@ -18887,13 +18872,13 @@
       <c r="B50" t="s">
         <v>1</v>
       </c>
-      <c r="C50" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D50" s="2" t="s">
+      <c r="C50" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="2" t="s">
         <v>986</v>
       </c>
       <c r="F50">
@@ -18908,7 +18893,7 @@
       <c r="I50" t="s">
         <v>5</v>
       </c>
-      <c r="J50" s="4">
+      <c r="J50" s="3">
         <v>7.5</v>
       </c>
       <c r="K50" t="s">
@@ -19186,13 +19171,13 @@
       <c r="B51" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D51" s="2" t="s">
+      <c r="C51" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="2" t="s">
         <v>986</v>
       </c>
       <c r="F51">
@@ -19207,7 +19192,7 @@
       <c r="I51" t="s">
         <v>5</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J51" s="3">
         <v>7.5</v>
       </c>
       <c r="K51" t="s">
@@ -19491,13 +19476,13 @@
       <c r="B52" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D52" s="2" t="s">
+      <c r="C52" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>986</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="2" t="s">
         <v>986</v>
       </c>
       <c r="F52">
@@ -19512,7 +19497,7 @@
       <c r="I52" t="s">
         <v>5</v>
       </c>
-      <c r="J52" s="4">
+      <c r="J52" s="3">
         <v>7.5</v>
       </c>
       <c r="K52" t="s">
@@ -19790,13 +19775,13 @@
       <c r="B53" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="C53" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="2" t="s">
         <v>1036</v>
       </c>
       <c r="F53">
@@ -19811,7 +19796,7 @@
       <c r="I53" t="s">
         <v>5</v>
       </c>
-      <c r="J53" s="4">
+      <c r="J53" s="3">
         <v>7.5</v>
       </c>
       <c r="K53" t="s">
@@ -20095,13 +20080,13 @@
       <c r="B54" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D54" s="2" t="s">
+      <c r="C54" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="E54" s="2" t="s">
         <v>1036</v>
       </c>
       <c r="F54">
@@ -20116,7 +20101,7 @@
       <c r="I54" t="s">
         <v>5</v>
       </c>
-      <c r="J54" s="4">
+      <c r="J54" s="3">
         <v>7.5</v>
       </c>
       <c r="K54" t="s">
@@ -20400,13 +20385,13 @@
       <c r="B55" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="8" t="s">
-        <v>1232</v>
-      </c>
-      <c r="D55" s="2" t="s">
+      <c r="C55" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>1036</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="2" t="s">
         <v>1036</v>
       </c>
       <c r="F55">
@@ -20421,7 +20406,7 @@
       <c r="I55" t="s">
         <v>5</v>
       </c>
-      <c r="J55" s="4">
+      <c r="J55" s="3">
         <v>7.5</v>
       </c>
       <c r="K55" t="s">
@@ -20705,13 +20690,13 @@
       <c r="B56" t="s">
         <v>1</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>1233</v>
-      </c>
-      <c r="D56" s="2" t="s">
+      <c r="C56" s="7" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>1083</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="2" t="s">
         <v>1083</v>
       </c>
       <c r="F56">
@@ -20726,7 +20711,7 @@
       <c r="I56" t="s">
         <v>5</v>
       </c>
-      <c r="J56" s="4">
+      <c r="J56" s="3">
         <v>7.5</v>
       </c>
       <c r="K56" t="s">
@@ -21010,13 +20995,13 @@
       <c r="B57" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="8" t="s">
-        <v>1233</v>
-      </c>
-      <c r="D57" s="2" t="s">
+      <c r="C57" s="7" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>1083</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="E57" s="2" t="s">
         <v>1083</v>
       </c>
       <c r="F57">
@@ -21031,7 +21016,7 @@
       <c r="I57" t="s">
         <v>5</v>
       </c>
-      <c r="J57" s="4">
+      <c r="J57" s="3">
         <v>7.5</v>
       </c>
       <c r="K57" t="s">
@@ -21315,13 +21300,13 @@
       <c r="B58" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="8" t="s">
-        <v>1233</v>
-      </c>
-      <c r="D58" s="2" t="s">
+      <c r="C58" s="7" t="s">
+        <v>1231</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>1083</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="E58" s="2" t="s">
         <v>1083</v>
       </c>
       <c r="F58">
@@ -21336,7 +21321,7 @@
       <c r="I58" t="s">
         <v>5</v>
       </c>
-      <c r="J58" s="4">
+      <c r="J58" s="3">
         <v>7.5</v>
       </c>
       <c r="K58" t="s">
@@ -21613,1096 +21598,8 @@
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D59" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA59">
-        <v>0.2107</v>
-      </c>
-      <c r="AG59">
-        <v>5.5199999999999999E-2</v>
-      </c>
-      <c r="AI59">
-        <v>2.7214</v>
-      </c>
-      <c r="AM59">
-        <v>1.5E-3</v>
-      </c>
-      <c r="AO59">
-        <v>6.4999999999999997E-3</v>
-      </c>
-      <c r="BC59">
-        <v>8.8999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="60" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D60" s="2">
-        <v>2</v>
-      </c>
-      <c r="AA60">
-        <v>0.21010000000000001</v>
-      </c>
-      <c r="AG60">
-        <v>4.5199999999999997E-2</v>
-      </c>
-      <c r="AI60">
-        <v>2.8073999999999999</v>
-      </c>
-      <c r="AM60">
-        <v>3.8E-3</v>
-      </c>
-      <c r="AO60">
-        <v>7.9000000000000008E-3</v>
-      </c>
-      <c r="BC60">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D61" s="2">
-        <v>3</v>
-      </c>
-      <c r="AA61">
-        <v>0.20530000000000001</v>
-      </c>
-      <c r="AG61">
-        <v>4.6300000000000001E-2</v>
-      </c>
-      <c r="AI61">
-        <v>2.7584</v>
-      </c>
-      <c r="AM61">
-        <v>1E-3</v>
-      </c>
-      <c r="AO61">
-        <v>7.1999999999999998E-3</v>
-      </c>
-      <c r="BC61">
-        <v>7.3000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="62" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D62" s="2">
-        <v>4</v>
-      </c>
-      <c r="AA62">
-        <v>0.17319999999999999</v>
-      </c>
-      <c r="AG62">
-        <v>4.0300000000000002E-2</v>
-      </c>
-      <c r="AI62">
-        <v>2.1461999999999999</v>
-      </c>
-      <c r="AM62">
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="AO62">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="BC62">
-        <v>6.8999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D63" s="2">
-        <v>5</v>
-      </c>
-      <c r="AA63">
-        <v>0.18140000000000001</v>
-      </c>
-      <c r="AG63">
-        <v>4.6800000000000001E-2</v>
-      </c>
-      <c r="AI63">
-        <v>2.3283</v>
-      </c>
-      <c r="AM63">
-        <v>5.3E-3</v>
-      </c>
-      <c r="AO63">
-        <v>6.1999999999999998E-3</v>
-      </c>
-      <c r="BC63">
-        <v>7.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D64" s="2">
-        <v>6</v>
-      </c>
-      <c r="AA64">
-        <v>0.18709999999999999</v>
-      </c>
-      <c r="AG64">
-        <v>4.65E-2</v>
-      </c>
-      <c r="AI64">
-        <v>2.5638999999999998</v>
-      </c>
-      <c r="AM64">
-        <v>2.2000000000000001E-3</v>
-      </c>
-      <c r="AO64">
-        <v>6.6E-3</v>
-      </c>
-      <c r="BC64">
-        <v>7.6E-3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D65" s="2">
-        <v>7</v>
-      </c>
-      <c r="AA65">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="AG65">
-        <v>4.6699999999999998E-2</v>
-      </c>
-      <c r="AI65">
-        <v>4.3887</v>
-      </c>
-      <c r="AM65">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="AO65">
-        <v>7.6E-3</v>
-      </c>
-      <c r="BC65">
-        <v>9.4999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="66" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D66" s="2">
-        <v>8</v>
-      </c>
-      <c r="AA66">
-        <v>0.1535</v>
-      </c>
-      <c r="AG66">
-        <v>3.3099999999999997E-2</v>
-      </c>
-      <c r="AI66">
-        <v>1.8684000000000001</v>
-      </c>
-      <c r="AM66">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="AO66">
-        <v>3.5999999999999999E-3</v>
-      </c>
-      <c r="BC66">
-        <v>4.3E-3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D67" s="2">
-        <v>9</v>
-      </c>
-      <c r="AA67">
-        <v>0.2306</v>
-      </c>
-      <c r="AG67">
-        <v>6.0900000000000003E-2</v>
-      </c>
-      <c r="AI67">
-        <v>3.6909999999999998</v>
-      </c>
-      <c r="AM67">
-        <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="AO67">
-        <v>7.7999999999999996E-3</v>
-      </c>
-      <c r="BC67">
-        <v>6.6E-3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D68" s="2">
-        <v>10</v>
-      </c>
-      <c r="AA68">
-        <v>0.15440000000000001</v>
-      </c>
-      <c r="AG68">
-        <v>3.44E-2</v>
-      </c>
-      <c r="AI68">
-        <v>2.0562</v>
-      </c>
-      <c r="AM68">
-        <v>2E-3</v>
-      </c>
-      <c r="AO68">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="BC68">
-        <v>4.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B69" t="s">
-        <v>1</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D69" s="2">
-        <v>11</v>
-      </c>
-      <c r="AA69">
-        <v>0.24179999999999999</v>
-      </c>
-      <c r="AG69">
-        <v>4.9500000000000002E-2</v>
-      </c>
-      <c r="AI69">
-        <v>3.3530000000000002</v>
-      </c>
-      <c r="AM69">
-        <v>1.5E-3</v>
-      </c>
-      <c r="AO69">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="BC69">
-        <v>1.06E-2</v>
-      </c>
-    </row>
-    <row r="70" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B70" t="s">
-        <v>1</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D70" s="2">
-        <v>12</v>
-      </c>
-      <c r="AA70">
-        <v>0.2336</v>
-      </c>
-      <c r="AG70">
-        <v>5.3499999999999999E-2</v>
-      </c>
-      <c r="AI70">
-        <v>2.7139000000000002</v>
-      </c>
-      <c r="AM70">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AO70">
-        <v>6.1999999999999998E-3</v>
-      </c>
-      <c r="BC70">
-        <v>8.8000000000000005E-3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D71" s="2">
-        <v>13</v>
-      </c>
-      <c r="AA71">
-        <v>0.22889999999999999</v>
-      </c>
-      <c r="AG71">
-        <v>4.7E-2</v>
-      </c>
-      <c r="AI71">
-        <v>3.1602999999999999</v>
-      </c>
-      <c r="AM71">
-        <v>3.8E-3</v>
-      </c>
-      <c r="AO71">
-        <v>5.8999999999999999E-3</v>
-      </c>
-      <c r="BC71">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="72" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D72" s="2">
-        <v>14</v>
-      </c>
-      <c r="AA72">
-        <v>0.2283</v>
-      </c>
-      <c r="AG72">
-        <v>4.9299999999999997E-2</v>
-      </c>
-      <c r="AI72">
-        <v>3.8910999999999998</v>
-      </c>
-      <c r="AM72">
-        <v>2.3E-3</v>
-      </c>
-      <c r="AO72">
-        <v>7.7999999999999996E-3</v>
-      </c>
-      <c r="BC72">
-        <v>9.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B73" t="s">
-        <v>1</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D73" s="2">
-        <v>15</v>
-      </c>
-      <c r="AA73">
-        <v>0.29070000000000001</v>
-      </c>
-      <c r="AG73">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="AI73">
-        <v>4.3101000000000003</v>
-      </c>
-      <c r="AM73">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AO73">
-        <v>5.7000000000000002E-3</v>
-      </c>
-      <c r="BC73">
-        <v>8.3000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B74" t="s">
-        <v>1</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D74" s="2">
-        <v>16</v>
-      </c>
-      <c r="AA74">
-        <v>0.1895</v>
-      </c>
-      <c r="AG74">
-        <v>3.9100000000000003E-2</v>
-      </c>
-      <c r="AI74">
-        <v>2.5089999999999999</v>
-      </c>
-      <c r="AM74">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="AO74">
-        <v>7.1999999999999998E-3</v>
-      </c>
-      <c r="BC74">
-        <v>8.5000000000000006E-3</v>
-      </c>
-    </row>
-    <row r="75" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B75" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D75" s="2">
-        <v>17</v>
-      </c>
-      <c r="AA75">
-        <v>0.26779999999999998</v>
-      </c>
-      <c r="AG75">
-        <v>5.16E-2</v>
-      </c>
-      <c r="AI75">
-        <v>4.1994999999999996</v>
-      </c>
-      <c r="AM75">
-        <v>3.8E-3</v>
-      </c>
-      <c r="AO75">
-        <v>5.8999999999999999E-3</v>
-      </c>
-      <c r="BC75">
-        <v>8.8000000000000005E-3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B76" t="s">
-        <v>1</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D76" s="2">
-        <v>18</v>
-      </c>
-      <c r="AA76">
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="AG76">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="AI76">
-        <v>4.2244000000000002</v>
-      </c>
-      <c r="AM76">
-        <v>1.6999999999999999E-3</v>
-      </c>
-      <c r="AO76">
-        <v>7.4000000000000003E-3</v>
-      </c>
-      <c r="BC76">
-        <v>1.2E-2</v>
-      </c>
-    </row>
-    <row r="77" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B77" t="s">
-        <v>1</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D77" s="2">
-        <v>19</v>
-      </c>
-      <c r="AA77">
-        <v>0.21179999999999999</v>
-      </c>
-      <c r="AG77">
-        <v>4.7899999999999998E-2</v>
-      </c>
-      <c r="AI77">
-        <v>2.7909000000000002</v>
-      </c>
-      <c r="AM77">
-        <v>4.3E-3</v>
-      </c>
-      <c r="AO77">
-        <v>6.6E-3</v>
-      </c>
-      <c r="BC77">
-        <v>7.7000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="78" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B78" t="s">
-        <v>1</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D78" s="2">
-        <v>20</v>
-      </c>
-      <c r="AA78">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="AG78">
-        <v>5.9900000000000002E-2</v>
-      </c>
-      <c r="AI78">
-        <v>3.7261000000000002</v>
-      </c>
-      <c r="AM78">
-        <v>2.3E-3</v>
-      </c>
-      <c r="AO78">
-        <v>7.1000000000000004E-3</v>
-      </c>
-      <c r="BC78">
-        <v>9.4000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B79" t="s">
-        <v>1</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D79" s="2">
-        <v>21</v>
-      </c>
-      <c r="AA79">
-        <v>0.25940000000000002</v>
-      </c>
-      <c r="AG79">
-        <v>5.9900000000000002E-2</v>
-      </c>
-      <c r="AI79">
-        <v>2.9661</v>
-      </c>
-      <c r="AM79">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="AO79">
-        <v>7.3000000000000001E-3</v>
-      </c>
-      <c r="BC79">
-        <v>1.11E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B80" t="s">
-        <v>1</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D80" s="2">
-        <v>22</v>
-      </c>
-      <c r="AA80">
-        <v>0.25490000000000002</v>
-      </c>
-      <c r="AG80">
-        <v>5.5199999999999999E-2</v>
-      </c>
-      <c r="AI80">
-        <v>3.6013000000000002</v>
-      </c>
-      <c r="AM80">
-        <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="AO80">
-        <v>8.0999999999999996E-3</v>
-      </c>
-      <c r="BC80">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="81" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B81" t="s">
-        <v>1</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D81" s="2">
-        <v>23</v>
-      </c>
-      <c r="AA81">
-        <v>0.248</v>
-      </c>
-      <c r="AG81">
-        <v>4.3299999999999998E-2</v>
-      </c>
-      <c r="AI81">
-        <v>3.2841</v>
-      </c>
-      <c r="AM81">
-        <v>5.8999999999999999E-3</v>
-      </c>
-      <c r="AO81">
-        <v>6.1999999999999998E-3</v>
-      </c>
-      <c r="BC81">
-        <v>6.1999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B82" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D82" s="2">
-        <v>24</v>
-      </c>
-      <c r="AA82">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="AG82">
-        <v>5.3499999999999999E-2</v>
-      </c>
-      <c r="AI82">
-        <v>3.7351000000000001</v>
-      </c>
-      <c r="AM82">
-        <v>1E-3</v>
-      </c>
-      <c r="AO82">
-        <v>6.3E-3</v>
-      </c>
-      <c r="BC82">
-        <v>9.4999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B83" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D83" s="2">
-        <v>25</v>
-      </c>
-      <c r="AA83">
-        <v>0.2712</v>
-      </c>
-      <c r="AG83">
-        <v>5.91E-2</v>
-      </c>
-      <c r="AI83">
-        <v>4.3178999999999998</v>
-      </c>
-      <c r="AM83">
-        <v>1.4E-3</v>
-      </c>
-      <c r="AO83">
-        <v>6.4000000000000003E-3</v>
-      </c>
-      <c r="BC83">
-        <v>8.0999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B84" t="s">
-        <v>1</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D84" s="2">
-        <v>26</v>
-      </c>
-      <c r="AA84">
-        <v>0.35709999999999997</v>
-      </c>
-      <c r="AG84">
-        <v>6.6600000000000006E-2</v>
-      </c>
-      <c r="AI84">
-        <v>4.7754000000000003</v>
-      </c>
-      <c r="AM84">
-        <v>1.5E-3</v>
-      </c>
-      <c r="AO84">
-        <v>7.1000000000000004E-3</v>
-      </c>
-      <c r="BC84">
-        <v>1.0999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="85" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B85" t="s">
-        <v>1</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D85" s="2">
-        <v>27</v>
-      </c>
-      <c r="AA85">
-        <v>0.29820000000000002</v>
-      </c>
-      <c r="AG85">
-        <v>5.4399999999999997E-2</v>
-      </c>
-      <c r="AI85">
-        <v>4.6767000000000003</v>
-      </c>
-      <c r="AM85">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="AO85">
-        <v>7.6E-3</v>
-      </c>
-      <c r="BC85">
-        <v>9.7000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B86" t="s">
-        <v>1</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D86" s="2">
-        <v>28</v>
-      </c>
-      <c r="AA86">
-        <v>0.18729999999999999</v>
-      </c>
-      <c r="AG86">
-        <v>3.6499999999999998E-2</v>
-      </c>
-      <c r="AI86">
-        <v>2.6261000000000001</v>
-      </c>
-      <c r="AM86">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="AO86">
-        <v>6.3E-3</v>
-      </c>
-      <c r="BC86">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B87" t="s">
-        <v>1</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D87" s="2">
-        <v>29</v>
-      </c>
-      <c r="AA87">
-        <v>0.2266</v>
-      </c>
-      <c r="AG87">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="AI87">
-        <v>3.4003000000000001</v>
-      </c>
-      <c r="AM87">
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="AO87">
-        <v>6.8999999999999999E-3</v>
-      </c>
-      <c r="BC87">
-        <v>8.8999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="88" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B88" t="s">
-        <v>1</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D88" s="2">
-        <v>30</v>
-      </c>
-      <c r="AA88">
-        <v>0.27450000000000002</v>
-      </c>
-      <c r="AG88">
-        <v>4.3900000000000002E-2</v>
-      </c>
-      <c r="AI88">
-        <v>3.1737000000000002</v>
-      </c>
-      <c r="AM88">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AO88">
-        <v>7.1999999999999998E-3</v>
-      </c>
-      <c r="BC88">
-        <v>8.8000000000000005E-3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B89" t="s">
-        <v>1</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D89" s="2">
-        <v>31</v>
-      </c>
-      <c r="AA89">
-        <v>0.24</v>
-      </c>
-      <c r="AG89">
-        <v>5.0099999999999999E-2</v>
-      </c>
-      <c r="AI89">
-        <v>2.7648999999999999</v>
-      </c>
-      <c r="AM89">
-        <v>5.1999999999999998E-3</v>
-      </c>
-      <c r="AO89">
-        <v>6.1999999999999998E-3</v>
-      </c>
-      <c r="BC89">
-        <v>7.7999999999999996E-3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B90" t="s">
-        <v>1</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D90" s="2">
-        <v>32</v>
-      </c>
-      <c r="AA90">
-        <v>0.29360000000000003</v>
-      </c>
-      <c r="AG90">
-        <v>6.3700000000000007E-2</v>
-      </c>
-      <c r="AI90">
-        <v>3.0266000000000002</v>
-      </c>
-      <c r="AM90">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="AO90">
-        <v>8.3000000000000001E-3</v>
-      </c>
-      <c r="BC90">
-        <v>1.14E-2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B91" t="s">
-        <v>1</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D91" s="2">
-        <v>33</v>
-      </c>
-      <c r="AA91">
-        <v>0.27860000000000001</v>
-      </c>
-      <c r="AG91">
-        <v>6.25E-2</v>
-      </c>
-      <c r="AI91">
-        <v>2.8744999999999998</v>
-      </c>
-      <c r="AM91">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="AO91">
-        <v>7.9000000000000008E-3</v>
-      </c>
-      <c r="BC91">
-        <v>1.1900000000000001E-2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:55" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B92" t="s">
-        <v>1</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>1224</v>
-      </c>
-      <c r="D92" s="2">
-        <v>34</v>
-      </c>
-      <c r="AA92">
-        <v>0.2772</v>
-      </c>
-      <c r="AG92">
-        <v>6.2700000000000006E-2</v>
-      </c>
-      <c r="AI92">
-        <v>3.0636999999999999</v>
-      </c>
-      <c r="AM92">
-        <v>3.0999999999999999E-3</v>
-      </c>
-      <c r="AO92">
-        <v>6.1000000000000004E-3</v>
-      </c>
-      <c r="BC92">
-        <v>1.2200000000000001E-2</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added combined PCA analysis
</commit_message>
<xml_diff>
--- a/results/palaepaphos/data/pxrf_PP.xlsx
+++ b/results/palaepaphos/data/pxrf_PP.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\R\MB\results\palaepaphos\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uine\Documents\R\MB\results\palaepaphos\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{595845D0-7112-4843-9053-C2EC6D0F5CBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="105" windowWidth="17715" windowHeight="15495"/>
+    <workbookView xWindow="1170" yWindow="105" windowWidth="13395" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5670" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5670" uniqueCount="1229">
   <si>
     <t>soil</t>
   </si>
@@ -3706,21 +3699,6 @@
     <t>Other name</t>
   </si>
   <si>
-    <t>Hadjuabudllah l1</t>
-  </si>
-  <si>
-    <t>Hadjuabudllah l2</t>
-  </si>
-  <si>
-    <t>Laona soil l1</t>
-  </si>
-  <si>
-    <t>Laona soil l2</t>
-  </si>
-  <si>
-    <t>Laona soil l3</t>
-  </si>
-  <si>
     <t>LA54:4</t>
   </si>
   <si>
@@ -3728,12 +3706,18 @@
   </si>
   <si>
     <t>LA54:7</t>
+  </si>
+  <si>
+    <t>Hadjuabudllah</t>
+  </si>
+  <si>
+    <t>Laona soil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4114,12 +4098,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CW58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B62" sqref="B62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4443,7 +4427,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1224</v>
+        <v>1227</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -4748,7 +4732,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>1224</v>
+        <v>1227</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -5047,7 +5031,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>1224</v>
+        <v>1227</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -5346,7 +5330,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>122</v>
@@ -5651,7 +5635,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>122</v>
@@ -5950,7 +5934,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>122</v>
@@ -6249,7 +6233,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>202</v>
@@ -6554,7 +6538,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>202</v>
@@ -6853,7 +6837,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>202</v>
@@ -7158,7 +7142,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>278</v>
@@ -7451,7 +7435,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>278</v>
@@ -7756,7 +7740,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>278</v>
@@ -8964,7 +8948,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>403</v>
@@ -9257,7 +9241,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>403</v>
@@ -9550,7 +9534,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>403</v>
@@ -9855,7 +9839,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>459</v>
@@ -10154,7 +10138,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>459</v>
@@ -10453,7 +10437,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>459</v>
@@ -11661,7 +11645,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>582</v>
@@ -11966,7 +11950,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>582</v>
@@ -12265,7 +12249,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>582</v>
@@ -12564,7 +12548,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>638</v>
@@ -12863,7 +12847,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>638</v>
@@ -13162,7 +13146,7 @@
         <v>1</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>638</v>
@@ -13461,7 +13445,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>691</v>
@@ -13760,7 +13744,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>691</v>
@@ -14059,7 +14043,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>691</v>
@@ -14358,7 +14342,7 @@
         <v>1</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>744</v>
@@ -14663,7 +14647,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>744</v>
@@ -14962,7 +14946,7 @@
         <v>1</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>744</v>
@@ -15261,7 +15245,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>792</v>
@@ -15560,7 +15544,7 @@
         <v>1</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>792</v>
@@ -15865,7 +15849,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>1229</v>
+        <v>1224</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>792</v>
@@ -16164,7 +16148,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>841</v>
@@ -16463,7 +16447,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>841</v>
@@ -16762,7 +16746,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>841</v>
@@ -17061,7 +17045,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>891</v>
@@ -17360,7 +17344,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>891</v>
@@ -17659,7 +17643,7 @@
         <v>1</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>891</v>
@@ -17964,7 +17948,7 @@
         <v>1</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>938</v>
@@ -18269,7 +18253,7 @@
         <v>1</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>938</v>
@@ -18574,7 +18558,7 @@
         <v>1</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>938</v>
@@ -18873,7 +18857,7 @@
         <v>1</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>986</v>
@@ -19172,7 +19156,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>986</v>
@@ -19477,7 +19461,7 @@
         <v>1</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>986</v>
@@ -19776,7 +19760,7 @@
         <v>1</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>1036</v>
@@ -20081,7 +20065,7 @@
         <v>1</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>1036</v>
@@ -20386,7 +20370,7 @@
         <v>1</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>1230</v>
+        <v>1225</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>1036</v>
@@ -20691,7 +20675,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>1231</v>
+        <v>1226</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>1083</v>
@@ -20996,7 +20980,7 @@
         <v>1</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>1231</v>
+        <v>1226</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>1083</v>
@@ -21301,7 +21285,7 @@
         <v>1</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>1231</v>
+        <v>1226</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>1083</v>

</xml_diff>